<commit_message>
Added results of Solid studies for R6-NoEndcone and R6-Encone
</commit_message>
<xml_diff>
--- a/R6TR/data/PrawieR5-Solid/PrawieR5-TR-CD.xlsx
+++ b/R6TR/data/PrawieR5-Solid/PrawieR5-TR-CD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t xml:space="preserve">Design Point 1</t>
   </si>
@@ -71,6 +71,9 @@
     <t xml:space="preserve">GG Force (Z) 4 [N]</t>
   </si>
   <si>
+    <t xml:space="preserve">Diameter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Area</t>
   </si>
   <si>
@@ -90,9 +93,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -210,15 +212,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,11 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,11 +439,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="89180710"/>
-        <c:axId val="12427507"/>
+        <c:axId val="27953769"/>
+        <c:axId val="85316207"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89180710"/>
+        <c:axId val="27953769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +506,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12427507"/>
+        <c:crossAx val="85316207"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,7 +514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12427507"/>
+        <c:axId val="85316207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89180710"/>
+        <c:crossAx val="27953769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -734,11 +736,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="19245605"/>
-        <c:axId val="37685585"/>
+        <c:axId val="85842056"/>
+        <c:axId val="14013782"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="19245605"/>
+        <c:axId val="85842056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +803,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37685585"/>
+        <c:crossAx val="14013782"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -809,7 +811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37685585"/>
+        <c:axId val="14013782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +874,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19245605"/>
+        <c:crossAx val="85842056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1031,11 +1033,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="85630142"/>
-        <c:axId val="18340598"/>
+        <c:axId val="65584634"/>
+        <c:axId val="47434720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85630142"/>
+        <c:axId val="65584634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1100,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18340598"/>
+        <c:crossAx val="47434720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1106,7 +1108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18340598"/>
+        <c:axId val="47434720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1171,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85630142"/>
+        <c:crossAx val="65584634"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1328,11 +1330,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="21758302"/>
-        <c:axId val="67476158"/>
+        <c:axId val="9610535"/>
+        <c:axId val="75250236"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="21758302"/>
+        <c:axId val="9610535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67476158"/>
+        <c:crossAx val="75250236"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1403,7 +1405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67476158"/>
+        <c:axId val="75250236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1468,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21758302"/>
+        <c:crossAx val="9610535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1505,9 +1507,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>307800</xdr:colOff>
+      <xdr:colOff>307440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1516,7 +1518,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9299520" cy="6499800"/>
+        <a:ext cx="9299160" cy="6499440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1540,9 +1542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>307800</xdr:colOff>
+      <xdr:colOff>307440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1551,7 +1553,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9299520" cy="6499800"/>
+        <a:ext cx="9299160" cy="6499440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1575,9 +1577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>307800</xdr:colOff>
+      <xdr:colOff>307440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1586,7 +1588,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9299520" cy="6499800"/>
+        <a:ext cx="9299160" cy="6499440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1610,9 +1612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>307800</xdr:colOff>
+      <xdr:colOff>307440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1621,7 +1623,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9299520" cy="6499800"/>
+        <a:ext cx="9299160" cy="6499440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1783,7 +1785,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1807,7 +1809,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1831,7 +1833,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1855,7 +1857,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1879,247 +1881,255 @@
   </sheetPr>
   <dimension ref="B2:L31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>-340</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>-306</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>-272</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>-238</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <v>-204</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>-170</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>-136</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="3" t="n">
         <v>-102</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="3" t="n">
         <v>-68</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="L3" s="3" t="n">
         <v>-34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>645.488345427925</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>477.972821235028</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>371.83544652822</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>285.495915111698</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <v>211.999155327958</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>149.526361984344</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <v>96.9557108507787</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <v>55.947181987926</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="4" t="n">
         <v>25.2462498458606</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <v>6.24831110123301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>-4.04309431067281</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>-4.99604060722259</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>-2.61077926369176</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>-2.54688500073786</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <v>-2.42182256364055</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <v>-1.34412843826086</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <v>-1.21184475742672</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="4" t="n">
         <v>-0.540341570570314</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="4" t="n">
         <v>-0.241146203575437</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <v>-0.0752800326411809</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>-645.469108745503</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>-477.934963582408</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>-371.823515760671</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>-285.476613321441</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>-211.978205735002</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>-149.513693269125</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>-96.9445811208729</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="4" t="n">
         <v>-55.9426618574675</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <v>-25.2444504333384</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>-6.24772994409624</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>-2.61032088180832</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>-3.28269318240765</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>-1.37144039823101</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>-2.10973178856196</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <v>-1.71936049013653</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>-1.40107685095104</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <v>-0.815153468668243</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="4" t="n">
         <v>-0.458148658020464</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="4" t="n">
         <v>-0.179975587246947</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="4" t="n">
         <v>-0.0394604628798226</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0.085</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <f aca="false">3.1415*0.085*0.085</f>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <f aca="false">3.1415*D14*D14</f>
         <v>0.0226973375</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="4" t="n">
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="n">
         <v>1.225</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <v>101300</v>
       </c>
     </row>
@@ -2130,218 +2140,218 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="5" t="n">
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" s="6" t="n">
         <v>0.9</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="6" t="n">
         <v>0.8</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="6" t="n">
         <v>0.7</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="G25" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" s="6" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="6" t="n">
         <v>0.4</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="L25" s="5" t="n">
+      <c r="L25" s="6" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="3" t="n">
         <v>-340</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="3" t="n">
         <v>-306</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="3" t="n">
         <v>-272</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="3" t="n">
         <v>-238</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="3" t="n">
         <v>-204</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="H26" s="3" t="n">
         <v>-170</v>
       </c>
-      <c r="I26" s="2" t="n">
+      <c r="I26" s="3" t="n">
         <v>-136</v>
       </c>
-      <c r="J26" s="2" t="n">
+      <c r="J26" s="3" t="n">
         <v>-102</v>
       </c>
-      <c r="K26" s="2" t="n">
+      <c r="K26" s="3" t="n">
         <v>-68</v>
       </c>
-      <c r="L26" s="2" t="n">
+      <c r="L26" s="3" t="n">
         <v>-34</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="4" t="n">
         <v>645.488345427925</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="4" t="n">
         <v>477.972821235028</v>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="E27" s="4" t="n">
         <v>371.83544652822</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="4" t="n">
         <v>285.495915111698</v>
       </c>
-      <c r="G27" s="3" t="n">
+      <c r="G27" s="4" t="n">
         <v>211.999155327958</v>
       </c>
-      <c r="H27" s="3" t="n">
+      <c r="H27" s="4" t="n">
         <v>149.526361984344</v>
       </c>
-      <c r="I27" s="3" t="n">
+      <c r="I27" s="4" t="n">
         <v>96.9557108507787</v>
       </c>
-      <c r="J27" s="3" t="n">
+      <c r="J27" s="4" t="n">
         <v>55.947181987926</v>
       </c>
-      <c r="K27" s="3" t="n">
+      <c r="K27" s="4" t="n">
         <v>25.2462498458606</v>
       </c>
-      <c r="L27" s="3" t="n">
+      <c r="L27" s="4" t="n">
         <v>6.24831110123301</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="4" t="n">
         <v>-4.04309431067281</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="4" t="n">
         <v>-4.99604060722259</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="E28" s="4" t="n">
         <v>-2.61077926369176</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>-2.54688500073786</v>
       </c>
-      <c r="G28" s="3" t="n">
+      <c r="G28" s="4" t="n">
         <v>-2.42182256364055</v>
       </c>
-      <c r="H28" s="3" t="n">
+      <c r="H28" s="4" t="n">
         <v>-1.34412843826086</v>
       </c>
-      <c r="I28" s="3" t="n">
+      <c r="I28" s="4" t="n">
         <v>-1.21184475742672</v>
       </c>
-      <c r="J28" s="3" t="n">
+      <c r="J28" s="4" t="n">
         <v>-0.540341570570314</v>
       </c>
-      <c r="K28" s="3" t="n">
+      <c r="K28" s="4" t="n">
         <v>-0.241146203575437</v>
       </c>
-      <c r="L28" s="3" t="n">
+      <c r="L28" s="4" t="n">
         <v>-0.0752800326411809</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="4" t="n">
         <v>-645.469108745503</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="4" t="n">
         <v>-477.934963582408</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="4" t="n">
         <v>-371.823515760671</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="4" t="n">
         <v>-285.476613321441</v>
       </c>
-      <c r="G29" s="3" t="n">
+      <c r="G29" s="4" t="n">
         <v>-211.978205735002</v>
       </c>
-      <c r="H29" s="3" t="n">
+      <c r="H29" s="4" t="n">
         <v>-149.513693269125</v>
       </c>
-      <c r="I29" s="3" t="n">
+      <c r="I29" s="4" t="n">
         <v>-96.9445811208729</v>
       </c>
-      <c r="J29" s="3" t="n">
+      <c r="J29" s="4" t="n">
         <v>-55.9426618574675</v>
       </c>
-      <c r="K29" s="3" t="n">
+      <c r="K29" s="4" t="n">
         <v>-25.2444504333384</v>
       </c>
-      <c r="L29" s="3" t="n">
+      <c r="L29" s="4" t="n">
         <v>-6.24772994409624</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="4" t="n">
         <v>-2.61032088180832</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="4" t="n">
         <v>-3.28269318240765</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="4" t="n">
         <v>-1.37144039823101</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>-2.10973178856196</v>
       </c>
-      <c r="G30" s="3" t="n">
+      <c r="G30" s="4" t="n">
         <v>-1.71936049013653</v>
       </c>
-      <c r="H30" s="3" t="n">
+      <c r="H30" s="4" t="n">
         <v>-1.40107685095104</v>
       </c>
-      <c r="I30" s="3" t="n">
+      <c r="I30" s="4" t="n">
         <v>-0.815153468668243</v>
       </c>
-      <c r="J30" s="3" t="n">
+      <c r="J30" s="4" t="n">
         <v>-0.458148658020464</v>
       </c>
-      <c r="K30" s="3" t="n">
+      <c r="K30" s="4" t="n">
         <v>-0.179975587246947</v>
       </c>
-      <c r="L30" s="3" t="n">
+      <c r="L30" s="4" t="n">
         <v>-0.0394604628798226</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="5" t="s">
-        <v>19</v>
+      <c r="B31" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C31" s="6" t="n">
         <f aca="false">2*C27/($D$15*$D$16*C26*C26)</f>

</xml_diff>